<commit_message>
Se añade la funcion aventura y una demo
</commit_message>
<xml_diff>
--- a/Mapa.xlsx
+++ b/Mapa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Espacios de trabajo\Phyton\Con lo colegas\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9AE721-3225-442C-B63B-A67157B80016}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEAE84B-A4E6-4FD6-A606-FB1624A6FE47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>x</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Hay unas huellas que van al norte</t>
+  </si>
+  <si>
+    <t>No hay nada por aquí</t>
+  </si>
+  <si>
+    <t>Hay un cartel que pone"Hola,que haces que no ves los jojos?"</t>
+  </si>
+  <si>
+    <t>Hay un cartel que pone"Hola Irene,ve mas al norte,puede que encuentres algo"</t>
   </si>
 </sst>
 </file>
@@ -363,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,6 +418,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se intenta añadir la opcion mapa de monstruos,el cual consiste en una semillas de monstruos que cada lugar tiene y el programa añadira estos al campo de batalla cuando esten en su ubicacion
</commit_message>
<xml_diff>
--- a/Mapa.xlsx
+++ b/Mapa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Espacios de trabajo\Phyton\Con lo colegas\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEAE84B-A4E6-4FD6-A606-FB1624A6FE47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAE9A8C-BBA0-4A0F-A070-D9081FAFC486}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
         <v>-1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -440,7 +440,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -454,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Se cambia la funcion de pmenu para que sea mas visible
</commit_message>
<xml_diff>
--- a/Mapa.xlsx
+++ b/Mapa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Espacios de trabajo\Phyton\Con lo colegas\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAE9A8C-BBA0-4A0F-A070-D9081FAFC486}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5032C04-C350-4B5A-AE4C-2B41C4179DA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -454,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>

</xml_diff>